<commit_message>
Fixed ahmed youssef total points
</commit_message>
<xml_diff>
--- a/sprints-documents/sprint2/Sprint 2 Backlog.xlsx
+++ b/sprints-documents/sprint2/Sprint 2 Backlog.xlsx
@@ -116,7 +116,7 @@
       <t xml:space="preserve"> Total: </t>
     </r>
     <r>
-      <t>120</t>
+      <t>123</t>
     </r>
   </si>
   <si>
@@ -141,7 +141,7 @@
       <t>Avg:</t>
     </r>
     <r>
-      <t xml:space="preserve"> 10.9</t>
+      <t xml:space="preserve"> 11.2</t>
     </r>
   </si>
   <si>
@@ -617,7 +617,7 @@
         <v>16</v>
       </c>
       <c r="K3" s="2">
-        <v>11.0</v>
+        <v>14.0</v>
       </c>
       <c r="L3" s="2">
         <v>3.0</v>

</xml_diff>

<commit_message>
added a missing update story
</commit_message>
<xml_diff>
--- a/sprints-documents/sprint2/Sprint 2 Backlog.xlsx
+++ b/sprints-documents/sprint2/Sprint 2 Backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="91">
   <si>
     <t>Unique ID</t>
   </si>
@@ -131,7 +131,7 @@
     </r>
   </si>
   <si>
-    <t>Update Case (Mongo)</t>
+    <t>Update Reviewer (Mongo)</t>
   </si>
   <si>
     <r>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Read Case (Mongo)</t>
+  </si>
+  <si>
+    <t>Update Case (Mongo)</t>
   </si>
   <si>
     <t>Delete Case (Mongo)</t>
@@ -960,7 +963,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" ht="16.5" customHeight="1">
       <c r="A19" s="2">
         <v>15.0</v>
       </c>
@@ -1044,6 +1047,9 @@
       <c r="A24" s="2">
         <v>19.0</v>
       </c>
+      <c r="B24" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C24" s="2">
         <v>1.0</v>
       </c>
@@ -1062,7 +1068,7 @@
         <v>20.0</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C25" s="2">
         <v>1.0</v>
@@ -1085,7 +1091,7 @@
         <v>21.0</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C27" s="2">
         <v>2.0</v>
@@ -1105,7 +1111,7 @@
         <v>22.0</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C28" s="2">
         <v>1.0</v>
@@ -1125,7 +1131,7 @@
         <v>23.0</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C29" s="2">
         <v>1.0</v>
@@ -1145,7 +1151,7 @@
         <v>24.0</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C30" s="2">
         <v>1.0</v>
@@ -1168,7 +1174,7 @@
         <v>25.0</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C32" s="2">
         <v>2.0</v>
@@ -1188,7 +1194,7 @@
         <v>26.0</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C33" s="2">
         <v>1.0</v>
@@ -1208,7 +1214,7 @@
         <v>27.0</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C34" s="2">
         <v>1.0</v>
@@ -1228,7 +1234,7 @@
         <v>28.0</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C35" s="2">
         <v>1.0</v>
@@ -1251,7 +1257,7 @@
         <v>29.0</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C37" s="2">
         <v>2.0</v>
@@ -1271,7 +1277,7 @@
         <v>30.0</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C38" s="2">
         <v>1.0</v>
@@ -1291,7 +1297,7 @@
         <v>31.0</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C39" s="2">
         <v>1.0</v>
@@ -1311,7 +1317,7 @@
         <v>32.0</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C40" s="2">
         <v>1.0</v>
@@ -1329,7 +1335,7 @@
     <row r="42">
       <c r="A42" s="16"/>
       <c r="B42" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43">
@@ -1342,10 +1348,10 @@
     </row>
     <row r="44">
       <c r="A44" s="15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C44" s="15">
         <v>8.0</v>
@@ -1362,10 +1368,10 @@
     </row>
     <row r="45">
       <c r="A45" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C45" s="15">
         <v>8.0</v>
@@ -1386,10 +1392,10 @@
     </row>
     <row r="47">
       <c r="A47" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C47" s="15">
         <v>5.0</v>
@@ -1410,10 +1416,10 @@
     </row>
     <row r="49">
       <c r="A49" s="15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C49" s="15">
         <v>5.0</v>
@@ -1434,10 +1440,10 @@
     </row>
     <row r="51">
       <c r="A51" s="15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C51" s="15">
         <v>5.0</v>
@@ -1454,10 +1460,10 @@
     </row>
     <row r="52">
       <c r="A52" s="15" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C52" s="15">
         <v>5.0</v>
@@ -1478,10 +1484,10 @@
     </row>
     <row r="54">
       <c r="A54" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C54" s="15">
         <v>5.0</v>
@@ -1498,10 +1504,10 @@
     </row>
     <row r="55">
       <c r="A55" s="15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C55" s="15">
         <v>5.0</v>
@@ -1523,10 +1529,10 @@
     </row>
     <row r="57">
       <c r="A57" s="15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C57" s="15">
         <v>5.0</v>
@@ -1543,10 +1549,10 @@
     </row>
     <row r="58">
       <c r="A58" s="15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C58" s="15">
         <v>5.0</v>
@@ -1566,10 +1572,10 @@
     </row>
     <row r="60">
       <c r="A60" s="15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C60" s="15">
         <v>5.0</v>
@@ -1591,10 +1597,10 @@
     </row>
     <row r="62">
       <c r="A62" s="15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C62" s="21">
         <v>5.0</v>
@@ -1615,10 +1621,10 @@
     </row>
     <row r="64">
       <c r="A64" s="15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C64" s="15">
         <v>8.0</v>
@@ -1639,10 +1645,10 @@
     </row>
     <row r="66">
       <c r="A66" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C66" s="15">
         <v>3.0</v>
@@ -1659,10 +1665,10 @@
     </row>
     <row r="67">
       <c r="A67" s="15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C67" s="15">
         <v>3.0</v>
@@ -1679,10 +1685,10 @@
     </row>
     <row r="68">
       <c r="A68" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C68" s="15">
         <v>3.0</v>

</xml_diff>